<commit_message>
updated data and rdf
</commit_message>
<xml_diff>
--- a/AutryPubDesc/AutryPubDesc.xlsx
+++ b/AutryPubDesc/AutryPubDesc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="450" yWindow="420" windowWidth="20760" windowHeight="9135"/>
+    <workbookView xWindow="450" yWindow="465" windowWidth="20760" windowHeight="9645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -816,7 +816,7 @@
   </si>
   <si>
     <t>Painting, &lt;em&gt;Once Upon a Time in the West&lt;/em&gt;, circa 1968.
-The painting is the original art created for Paramount Picture's Swedish movie poster "Harmonica En Hamnare."</t>
+This painting is the original artwork created for Paramount Picture's Swedish movie poster "Harmonica En Hamnare."</t>
   </si>
   <si>
     <t>2008.9.1</t>
@@ -854,7 +854,7 @@
     <t>2008.48.1</t>
   </si>
   <si>
-    <t>Painting by Franz Arthur Bischoff, &lt;em&gt;The Docks at San Pedro&lt;/em&gt;, 1864-1929.</t>
+    <t>Painting by Franz Arthur Bischoff, &lt;em&gt;The Docks at San Pedro&lt;/em&gt;, probably circa 1900.</t>
   </si>
   <si>
     <t>2008.59.1</t>
@@ -941,7 +941,7 @@
     <t>2012.37.2</t>
   </si>
   <si>
-    <t>Painting by Eanger Irving Course, &lt;em&gt;The Tom-Tom Maker&lt;/em&gt;. Signed bottom left corner.</t>
+    <t>Painting by Eanger Irving Couse, &lt;em&gt;The Tom-Tom Maker&lt;/em&gt;. Signed bottom left corner.</t>
   </si>
   <si>
     <t>2012.37.3</t>
@@ -1053,8 +1053,8 @@
   </si>
   <si>
     <t>Sculpture by Joe Beeler, &lt;em&gt;Prairie Madonna&lt;/em&gt;.  
-Inscribed at back: &lt;em&gt;JOE BEELER CA&lt;/em&gt;
-Stamped at back: &lt;em&gt;BRONZE/SMITH 18/35.&lt;/em&gt;</t>
+Inscribed back: &lt;em&gt;JOE BEELER CA&lt;/em&gt;
+Stamped back: &lt;em&gt;BRONZE/SMITH 18/35.&lt;/em&gt;</t>
   </si>
   <si>
     <t>2012.37.24</t>
@@ -1188,7 +1188,7 @@
     <t>2014.34.1</t>
   </si>
   <si>
-    <t>Painting by Billy Schenck, &lt;em&gt;A River Runs Through It&lt;/em&gt;, 2011.</t>
+    <t>Painting by Bill Schenck, &lt;em&gt;A River Runs Through It&lt;/em&gt;, 2011.</t>
   </si>
   <si>
     <t>2015.5.1</t>
@@ -1626,7 +1626,7 @@
   <dimension ref="A1:B194"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>